<commit_message>
página de dashboard pronta e planilha de riscos atualizada
</commit_message>
<xml_diff>
--- a/documentos/planilha de riscos/planilia de risco.xlsx
+++ b/documentos/planilha de riscos/planilia de risco.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriel alvares\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabriel alvares\Desktop\band tec\disciplinas 1S\Z_projeto P.I 2ªSPRINT\CyberLife\documentos\planilha de riscos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1B41584-E738-4B57-96DB-59E46EC28206}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5A5C65-7E31-41CF-B769-735B9A63B6D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CA107832-A519-475E-BDB5-D3389EB7364C}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>id</t>
   </si>
@@ -58,10 +58,6 @@
   <si>
     <t>FALTA DE COMPROMETIMENTO DE UM OU MAIS 
 INTEGRANTES DO GRUPO</t>
-  </si>
-  <si>
-    <t>DESENTENDIMENTOS ENTRE OS INTEGRANTES POR AVERSÃO 
-A IDEIAS ATRAPALHANDO O PRECESSO DE DESENVOLVIMENTO DO PROJETO</t>
   </si>
   <si>
     <t>FALHAS NA SEGURANÇA 
@@ -95,6 +91,49 @@
 1- Baixo 
 2- Médio 
 3- Alto</t>
+  </si>
+  <si>
+    <t>mitigar</t>
+  </si>
+  <si>
+    <t>todos estarem
+integrados com
+o projeto</t>
+  </si>
+  <si>
+    <t>evitar</t>
+  </si>
+  <si>
+    <t>alinhando todos os 
+integrantes</t>
+  </si>
+  <si>
+    <t>DESENTENDIMENTOS ENTRE OS INTEGRANTES POR AVERSÃO 
+AS IDEIAS ATRAPALHANDO O PRECESSO DE DESENVOLVIMENTO DO PROJETO</t>
+  </si>
+  <si>
+    <t>conversar e tentar entrar
+em um consenso</t>
+  </si>
+  <si>
+    <t>checagem de progresso periódicamente</t>
+  </si>
+  <si>
+    <t>evitar/mitigar</t>
+  </si>
+  <si>
+    <t>evitar: conversar ao máximo nas checagens
+mitigar: elaborar um protótipo</t>
+  </si>
+  <si>
+    <t>ter uma boa segurança no software do projeto</t>
+  </si>
+  <si>
+    <t>contrato de segurança com 
+os funcionários/clientes</t>
+  </si>
+  <si>
+    <t>utilizando equipamentos de alta qualidade e máxima proteção</t>
   </si>
 </sst>
 </file>
@@ -175,22 +214,26 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,7 +550,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E26B82CA-7C86-4DA4-83DE-52D643AE135C}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -517,182 +562,215 @@
     <col min="4" max="4" width="32.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>2</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="5">
         <v>2</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:7" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="F2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <v>3</v>
       </c>
       <c r="E3" s="6">
         <v>3</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" ht="60.75" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="B4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2">
         <v>3</v>
       </c>
       <c r="E4" s="7">
         <v>9</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="1">
+      <c r="B5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <v>3</v>
       </c>
       <c r="E5" s="6">
         <v>3</v>
       </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2">
         <v>2</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>3</v>
       </c>
       <c r="E6" s="7">
         <v>6</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:7" ht="45.75" x14ac:dyDescent="0.25">
+      <c r="F6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="B7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2">
         <v>1</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>3</v>
       </c>
       <c r="E7" s="6">
         <v>3</v>
       </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:7" ht="45.75" x14ac:dyDescent="0.25">
+      <c r="F7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="1">
+      <c r="B8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2">
         <v>1</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="2">
         <v>3</v>
       </c>
       <c r="E8" s="6">
         <v>3</v>
       </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:7" ht="30.75" x14ac:dyDescent="0.25">
+      <c r="F8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="1">
+      <c r="B9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2">
         <v>1</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <v>3</v>
       </c>
       <c r="E9" s="6">
         <v>3</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+      <c r="F9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>